<commit_message>
added appendix to document
</commit_message>
<xml_diff>
--- a/latex/robotsDOF.xlsx
+++ b/latex/robotsDOF.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14040" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="Chart2" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="robotsDOF" localSheetId="2">Sheet1!$B$1:$J$181</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="270">
   <si>
     <t>Robot</t>
   </si>
@@ -844,16 +845,41 @@
   </si>
   <si>
     <t>offset</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>\\</t>
+  </si>
+  <si>
+    <t>\hline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -876,13 +902,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="15">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2599,11 +2653,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1828902040"/>
-        <c:axId val="1828899048"/>
+        <c:axId val="2067057016"/>
+        <c:axId val="2067059800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1828902040"/>
+        <c:axId val="2067057016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2613,12 +2667,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1828899048"/>
+        <c:crossAx val="2067059800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1828899048"/>
+        <c:axId val="2067059800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2629,13 +2683,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1828902040"/>
+        <c:crossAx val="2067057016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3794,8 +3849,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1815183672"/>
-        <c:axId val="1815180680"/>
+        <c:axId val="2067109544"/>
+        <c:axId val="2067112536"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -4347,11 +4402,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1815174344"/>
-        <c:axId val="1815177640"/>
+        <c:axId val="2067118872"/>
+        <c:axId val="2067115576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1815183672"/>
+        <c:axId val="2067109544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4361,12 +4416,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1815180680"/>
+        <c:crossAx val="2067112536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1815180680"/>
+        <c:axId val="2067112536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4377,12 +4432,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1815183672"/>
+        <c:crossAx val="2067109544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1815177640"/>
+        <c:axId val="2067115576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4392,12 +4447,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1815174344"/>
+        <c:crossAx val="2067118872"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1815174344"/>
+        <c:axId val="2067118872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4408,13 +4463,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1815177640"/>
+        <c:crossAx val="2067115576"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4440,7 +4496,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4479,7 +4535,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8582121" cy="5830455"/>
+    <xdr:ext cx="8578725" cy="5827059"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -5254,7 +5310,7 @@
   <dimension ref="A1:O181"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9152,4 +9208,4196 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G181"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E2">
+        <v>2009</v>
+      </c>
+      <c r="F2" t="s">
+        <v>268</v>
+      </c>
+      <c r="G2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3">
+        <v>1985</v>
+      </c>
+      <c r="F3" t="s">
+        <v>268</v>
+      </c>
+      <c r="G3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E4">
+        <v>1999</v>
+      </c>
+      <c r="F4" t="s">
+        <v>268</v>
+      </c>
+      <c r="G4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E5">
+        <v>1999</v>
+      </c>
+      <c r="F5" t="s">
+        <v>268</v>
+      </c>
+      <c r="G5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C6">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>267</v>
+      </c>
+      <c r="E6">
+        <v>1999</v>
+      </c>
+      <c r="F6" t="s">
+        <v>268</v>
+      </c>
+      <c r="G6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>228</v>
+      </c>
+      <c r="B7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E7">
+        <v>2010</v>
+      </c>
+      <c r="F7" t="s">
+        <v>268</v>
+      </c>
+      <c r="G7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C8">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>267</v>
+      </c>
+      <c r="E8">
+        <v>2005</v>
+      </c>
+      <c r="F8" t="s">
+        <v>268</v>
+      </c>
+      <c r="G8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>267</v>
+      </c>
+      <c r="E9">
+        <v>1998</v>
+      </c>
+      <c r="F9" t="s">
+        <v>268</v>
+      </c>
+      <c r="G9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>267</v>
+      </c>
+      <c r="C10">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>267</v>
+      </c>
+      <c r="E10">
+        <v>1986</v>
+      </c>
+      <c r="F10" t="s">
+        <v>268</v>
+      </c>
+      <c r="G10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B11" t="s">
+        <v>267</v>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>267</v>
+      </c>
+      <c r="E11">
+        <v>2011</v>
+      </c>
+      <c r="F11" t="s">
+        <v>268</v>
+      </c>
+      <c r="G11" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C12">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>267</v>
+      </c>
+      <c r="E12">
+        <v>2001</v>
+      </c>
+      <c r="F12" t="s">
+        <v>268</v>
+      </c>
+      <c r="G12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" t="s">
+        <v>267</v>
+      </c>
+      <c r="C13">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>267</v>
+      </c>
+      <c r="E13">
+        <v>2005</v>
+      </c>
+      <c r="F13" t="s">
+        <v>268</v>
+      </c>
+      <c r="G13" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" t="s">
+        <v>267</v>
+      </c>
+      <c r="C14">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>267</v>
+      </c>
+      <c r="E14">
+        <v>2000</v>
+      </c>
+      <c r="F14" t="s">
+        <v>268</v>
+      </c>
+      <c r="G14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>267</v>
+      </c>
+      <c r="C15">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>267</v>
+      </c>
+      <c r="E15">
+        <v>2008</v>
+      </c>
+      <c r="F15" t="s">
+        <v>268</v>
+      </c>
+      <c r="G15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>267</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>267</v>
+      </c>
+      <c r="E16">
+        <v>1960</v>
+      </c>
+      <c r="F16" t="s">
+        <v>268</v>
+      </c>
+      <c r="G16" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" t="s">
+        <v>267</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>267</v>
+      </c>
+      <c r="E17">
+        <v>1940</v>
+      </c>
+      <c r="F17" t="s">
+        <v>268</v>
+      </c>
+      <c r="G17" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>267</v>
+      </c>
+      <c r="E18">
+        <v>1979</v>
+      </c>
+      <c r="F18" t="s">
+        <v>268</v>
+      </c>
+      <c r="G18" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>267</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>267</v>
+      </c>
+      <c r="E19">
+        <v>2005</v>
+      </c>
+      <c r="F19" t="s">
+        <v>268</v>
+      </c>
+      <c r="G19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>267</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>267</v>
+      </c>
+      <c r="E20">
+        <v>2007</v>
+      </c>
+      <c r="F20" t="s">
+        <v>268</v>
+      </c>
+      <c r="G20" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>194</v>
+      </c>
+      <c r="B21" t="s">
+        <v>267</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>267</v>
+      </c>
+      <c r="E21">
+        <v>1996</v>
+      </c>
+      <c r="F21" t="s">
+        <v>268</v>
+      </c>
+      <c r="G21" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" t="s">
+        <v>267</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>267</v>
+      </c>
+      <c r="E22">
+        <v>1995</v>
+      </c>
+      <c r="F22" t="s">
+        <v>268</v>
+      </c>
+      <c r="G22" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>267</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>267</v>
+      </c>
+      <c r="E23">
+        <v>2001</v>
+      </c>
+      <c r="F23" t="s">
+        <v>268</v>
+      </c>
+      <c r="G23" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="s">
+        <v>267</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>267</v>
+      </c>
+      <c r="E24">
+        <v>1942</v>
+      </c>
+      <c r="F24" t="s">
+        <v>268</v>
+      </c>
+      <c r="G24" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" t="s">
+        <v>267</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>267</v>
+      </c>
+      <c r="E25">
+        <v>1981</v>
+      </c>
+      <c r="F25" t="s">
+        <v>268</v>
+      </c>
+      <c r="G25" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B26" t="s">
+        <v>267</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>267</v>
+      </c>
+      <c r="E26">
+        <v>2015</v>
+      </c>
+      <c r="F26" t="s">
+        <v>268</v>
+      </c>
+      <c r="G26" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>216</v>
+      </c>
+      <c r="B27" t="s">
+        <v>267</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>267</v>
+      </c>
+      <c r="E27">
+        <v>1999</v>
+      </c>
+      <c r="F27" t="s">
+        <v>268</v>
+      </c>
+      <c r="G27" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
+        <v>267</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>267</v>
+      </c>
+      <c r="E28">
+        <v>2012</v>
+      </c>
+      <c r="F28" t="s">
+        <v>268</v>
+      </c>
+      <c r="G28" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C29">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>267</v>
+      </c>
+      <c r="E29">
+        <v>2004</v>
+      </c>
+      <c r="F29" t="s">
+        <v>268</v>
+      </c>
+      <c r="G29" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>217</v>
+      </c>
+      <c r="B30" t="s">
+        <v>267</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>267</v>
+      </c>
+      <c r="E30">
+        <v>1999</v>
+      </c>
+      <c r="F30" t="s">
+        <v>268</v>
+      </c>
+      <c r="G30" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" t="s">
+        <v>267</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>267</v>
+      </c>
+      <c r="E31">
+        <v>1990</v>
+      </c>
+      <c r="F31" t="s">
+        <v>268</v>
+      </c>
+      <c r="G31" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>267</v>
+      </c>
+      <c r="C32">
+        <v>28</v>
+      </c>
+      <c r="D32" t="s">
+        <v>267</v>
+      </c>
+      <c r="E32">
+        <v>1998</v>
+      </c>
+      <c r="F32" t="s">
+        <v>268</v>
+      </c>
+      <c r="G32" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>267</v>
+      </c>
+      <c r="C33">
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
+        <v>267</v>
+      </c>
+      <c r="E33">
+        <v>2010</v>
+      </c>
+      <c r="F33" t="s">
+        <v>268</v>
+      </c>
+      <c r="G33" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
+        <v>267</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>267</v>
+      </c>
+      <c r="E34">
+        <v>2010</v>
+      </c>
+      <c r="F34" t="s">
+        <v>268</v>
+      </c>
+      <c r="G34" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" t="s">
+        <v>267</v>
+      </c>
+      <c r="C35">
+        <v>28</v>
+      </c>
+      <c r="D35" t="s">
+        <v>267</v>
+      </c>
+      <c r="E35">
+        <v>1992</v>
+      </c>
+      <c r="F35" t="s">
+        <v>268</v>
+      </c>
+      <c r="G35" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>267</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>267</v>
+      </c>
+      <c r="E36">
+        <v>2002</v>
+      </c>
+      <c r="F36" t="s">
+        <v>268</v>
+      </c>
+      <c r="G36" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>267</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
+        <v>267</v>
+      </c>
+      <c r="E37">
+        <v>2008</v>
+      </c>
+      <c r="F37" t="s">
+        <v>268</v>
+      </c>
+      <c r="G37" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" t="s">
+        <v>267</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>267</v>
+      </c>
+      <c r="E38">
+        <v>1986</v>
+      </c>
+      <c r="F38" t="s">
+        <v>268</v>
+      </c>
+      <c r="G38" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" t="s">
+        <v>267</v>
+      </c>
+      <c r="C39">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>267</v>
+      </c>
+      <c r="E39">
+        <v>1987</v>
+      </c>
+      <c r="F39" t="s">
+        <v>268</v>
+      </c>
+      <c r="G39" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" t="s">
+        <v>267</v>
+      </c>
+      <c r="C40">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
+        <v>267</v>
+      </c>
+      <c r="E40">
+        <v>1989</v>
+      </c>
+      <c r="F40" t="s">
+        <v>268</v>
+      </c>
+      <c r="G40" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" t="s">
+        <v>267</v>
+      </c>
+      <c r="C41">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>267</v>
+      </c>
+      <c r="E41">
+        <v>1991</v>
+      </c>
+      <c r="F41" t="s">
+        <v>268</v>
+      </c>
+      <c r="G41" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>149</v>
+      </c>
+      <c r="B42" t="s">
+        <v>267</v>
+      </c>
+      <c r="C42">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s">
+        <v>267</v>
+      </c>
+      <c r="E42">
+        <v>1991</v>
+      </c>
+      <c r="F42" t="s">
+        <v>268</v>
+      </c>
+      <c r="G42" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" t="s">
+        <v>267</v>
+      </c>
+      <c r="C43">
+        <v>12</v>
+      </c>
+      <c r="D43" t="s">
+        <v>267</v>
+      </c>
+      <c r="E43">
+        <v>1992</v>
+      </c>
+      <c r="F43" t="s">
+        <v>268</v>
+      </c>
+      <c r="G43" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" t="s">
+        <v>267</v>
+      </c>
+      <c r="C44">
+        <v>12</v>
+      </c>
+      <c r="D44" t="s">
+        <v>267</v>
+      </c>
+      <c r="E44">
+        <v>1993</v>
+      </c>
+      <c r="F44" t="s">
+        <v>268</v>
+      </c>
+      <c r="G44" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>196</v>
+      </c>
+      <c r="B45" t="s">
+        <v>267</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>267</v>
+      </c>
+      <c r="E45">
+        <v>1996</v>
+      </c>
+      <c r="F45" t="s">
+        <v>268</v>
+      </c>
+      <c r="G45" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" t="s">
+        <v>267</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>267</v>
+      </c>
+      <c r="E46">
+        <v>1949</v>
+      </c>
+      <c r="F46" t="s">
+        <v>268</v>
+      </c>
+      <c r="G46" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s">
+        <v>267</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
+        <v>267</v>
+      </c>
+      <c r="E47">
+        <v>1948</v>
+      </c>
+      <c r="F47" t="s">
+        <v>268</v>
+      </c>
+      <c r="G47" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>163</v>
+      </c>
+      <c r="B48" t="s">
+        <v>267</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>267</v>
+      </c>
+      <c r="E48">
+        <v>2000</v>
+      </c>
+      <c r="F48" t="s">
+        <v>268</v>
+      </c>
+      <c r="G48" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>212</v>
+      </c>
+      <c r="B49" t="s">
+        <v>267</v>
+      </c>
+      <c r="C49">
+        <v>19</v>
+      </c>
+      <c r="D49" t="s">
+        <v>267</v>
+      </c>
+      <c r="E49">
+        <v>1999</v>
+      </c>
+      <c r="F49" t="s">
+        <v>268</v>
+      </c>
+      <c r="G49" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>203</v>
+      </c>
+      <c r="B50" t="s">
+        <v>267</v>
+      </c>
+      <c r="C50">
+        <v>20</v>
+      </c>
+      <c r="D50" t="s">
+        <v>267</v>
+      </c>
+      <c r="E50">
+        <v>1999</v>
+      </c>
+      <c r="F50" t="s">
+        <v>268</v>
+      </c>
+      <c r="G50" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>208</v>
+      </c>
+      <c r="B51" t="s">
+        <v>267</v>
+      </c>
+      <c r="C51">
+        <v>16</v>
+      </c>
+      <c r="D51" t="s">
+        <v>267</v>
+      </c>
+      <c r="E51">
+        <v>2000</v>
+      </c>
+      <c r="F51" t="s">
+        <v>268</v>
+      </c>
+      <c r="G51" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>205</v>
+      </c>
+      <c r="B52" t="s">
+        <v>267</v>
+      </c>
+      <c r="C52">
+        <v>15</v>
+      </c>
+      <c r="D52" t="s">
+        <v>267</v>
+      </c>
+      <c r="E52">
+        <v>1999</v>
+      </c>
+      <c r="F52" t="s">
+        <v>268</v>
+      </c>
+      <c r="G52" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>206</v>
+      </c>
+      <c r="B53" t="s">
+        <v>267</v>
+      </c>
+      <c r="C53">
+        <v>15</v>
+      </c>
+      <c r="D53" t="s">
+        <v>267</v>
+      </c>
+      <c r="E53">
+        <v>2001</v>
+      </c>
+      <c r="F53" t="s">
+        <v>268</v>
+      </c>
+      <c r="G53" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>207</v>
+      </c>
+      <c r="B54" t="s">
+        <v>267</v>
+      </c>
+      <c r="C54">
+        <v>15</v>
+      </c>
+      <c r="D54" t="s">
+        <v>267</v>
+      </c>
+      <c r="E54">
+        <v>2001</v>
+      </c>
+      <c r="F54" t="s">
+        <v>268</v>
+      </c>
+      <c r="G54" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>213</v>
+      </c>
+      <c r="B55" t="s">
+        <v>267</v>
+      </c>
+      <c r="C55">
+        <v>20</v>
+      </c>
+      <c r="D55" t="s">
+        <v>267</v>
+      </c>
+      <c r="E55">
+        <v>2003</v>
+      </c>
+      <c r="F55" t="s">
+        <v>268</v>
+      </c>
+      <c r="G55" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>214</v>
+      </c>
+      <c r="B56" t="s">
+        <v>267</v>
+      </c>
+      <c r="C56">
+        <v>20</v>
+      </c>
+      <c r="D56" t="s">
+        <v>267</v>
+      </c>
+      <c r="E56">
+        <v>2004</v>
+      </c>
+      <c r="F56" t="s">
+        <v>268</v>
+      </c>
+      <c r="G56" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>215</v>
+      </c>
+      <c r="B57" t="s">
+        <v>267</v>
+      </c>
+      <c r="C57">
+        <v>20</v>
+      </c>
+      <c r="D57" t="s">
+        <v>267</v>
+      </c>
+      <c r="E57">
+        <v>2005</v>
+      </c>
+      <c r="F57" t="s">
+        <v>268</v>
+      </c>
+      <c r="G57" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>254</v>
+      </c>
+      <c r="B58" t="s">
+        <v>267</v>
+      </c>
+      <c r="C58">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
+        <v>267</v>
+      </c>
+      <c r="E58">
+        <v>1973</v>
+      </c>
+      <c r="F58" t="s">
+        <v>268</v>
+      </c>
+      <c r="G58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>36</v>
+      </c>
+      <c r="B59" t="s">
+        <v>267</v>
+      </c>
+      <c r="C59">
+        <v>20</v>
+      </c>
+      <c r="D59" t="s">
+        <v>267</v>
+      </c>
+      <c r="E59">
+        <v>2003</v>
+      </c>
+      <c r="F59" t="s">
+        <v>268</v>
+      </c>
+      <c r="G59" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>111</v>
+      </c>
+      <c r="B60" t="s">
+        <v>267</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60" t="s">
+        <v>267</v>
+      </c>
+      <c r="E60">
+        <v>1969</v>
+      </c>
+      <c r="F60" t="s">
+        <v>268</v>
+      </c>
+      <c r="G60" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" t="s">
+        <v>267</v>
+      </c>
+      <c r="C61">
+        <v>5</v>
+      </c>
+      <c r="D61" t="s">
+        <v>267</v>
+      </c>
+      <c r="E61">
+        <v>1973</v>
+      </c>
+      <c r="F61" t="s">
+        <v>268</v>
+      </c>
+      <c r="G61" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62" t="s">
+        <v>267</v>
+      </c>
+      <c r="C62">
+        <v>9</v>
+      </c>
+      <c r="D62" t="s">
+        <v>267</v>
+      </c>
+      <c r="E62">
+        <v>2003</v>
+      </c>
+      <c r="F62" t="s">
+        <v>268</v>
+      </c>
+      <c r="G62" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63" t="s">
+        <v>267</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>267</v>
+      </c>
+      <c r="E63">
+        <v>1929</v>
+      </c>
+      <c r="F63" t="s">
+        <v>268</v>
+      </c>
+      <c r="G63" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" t="s">
+        <v>267</v>
+      </c>
+      <c r="C64">
+        <v>30</v>
+      </c>
+      <c r="D64" t="s">
+        <v>267</v>
+      </c>
+      <c r="E64">
+        <v>2005</v>
+      </c>
+      <c r="F64" t="s">
+        <v>268</v>
+      </c>
+      <c r="G64" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>230</v>
+      </c>
+      <c r="B65" t="s">
+        <v>267</v>
+      </c>
+      <c r="C65">
+        <v>20</v>
+      </c>
+      <c r="D65" t="s">
+        <v>267</v>
+      </c>
+      <c r="E65">
+        <v>2010</v>
+      </c>
+      <c r="F65" t="s">
+        <v>268</v>
+      </c>
+      <c r="G65" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>92</v>
+      </c>
+      <c r="B66" t="s">
+        <v>267</v>
+      </c>
+      <c r="C66">
+        <v>5</v>
+      </c>
+      <c r="D66" t="s">
+        <v>267</v>
+      </c>
+      <c r="E66">
+        <v>1949</v>
+      </c>
+      <c r="F66" t="s">
+        <v>268</v>
+      </c>
+      <c r="G66" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s">
+        <v>267</v>
+      </c>
+      <c r="E67">
+        <v>1944</v>
+      </c>
+      <c r="F67" t="s">
+        <v>268</v>
+      </c>
+      <c r="G67" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>233</v>
+      </c>
+      <c r="B68" t="s">
+        <v>267</v>
+      </c>
+      <c r="C68">
+        <v>26</v>
+      </c>
+      <c r="D68" t="s">
+        <v>267</v>
+      </c>
+      <c r="E68">
+        <v>1965</v>
+      </c>
+      <c r="F68" t="s">
+        <v>268</v>
+      </c>
+      <c r="G68" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>40</v>
+      </c>
+      <c r="B69" t="s">
+        <v>267</v>
+      </c>
+      <c r="C69">
+        <v>35</v>
+      </c>
+      <c r="D69" t="s">
+        <v>267</v>
+      </c>
+      <c r="E69">
+        <v>2011</v>
+      </c>
+      <c r="F69" t="s">
+        <v>268</v>
+      </c>
+      <c r="G69" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>105</v>
+      </c>
+      <c r="B70" t="s">
+        <v>267</v>
+      </c>
+      <c r="C70">
+        <v>24</v>
+      </c>
+      <c r="D70" t="s">
+        <v>267</v>
+      </c>
+      <c r="E70">
+        <v>1965</v>
+      </c>
+      <c r="F70" t="s">
+        <v>268</v>
+      </c>
+      <c r="G70" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
+        <v>135</v>
+      </c>
+      <c r="B71" t="s">
+        <v>267</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71" t="s">
+        <v>267</v>
+      </c>
+      <c r="E71">
+        <v>1982</v>
+      </c>
+      <c r="F71" t="s">
+        <v>268</v>
+      </c>
+      <c r="G71" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72" t="s">
+        <v>267</v>
+      </c>
+      <c r="C72">
+        <v>28</v>
+      </c>
+      <c r="D72" t="s">
+        <v>267</v>
+      </c>
+      <c r="E72">
+        <v>1997</v>
+      </c>
+      <c r="F72" t="s">
+        <v>268</v>
+      </c>
+      <c r="G72" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
+        <v>44</v>
+      </c>
+      <c r="B73" t="s">
+        <v>267</v>
+      </c>
+      <c r="C73">
+        <v>30</v>
+      </c>
+      <c r="D73" t="s">
+        <v>267</v>
+      </c>
+      <c r="E73">
+        <v>2002</v>
+      </c>
+      <c r="F73" t="s">
+        <v>268</v>
+      </c>
+      <c r="G73" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
+        <v>43</v>
+      </c>
+      <c r="B74" t="s">
+        <v>267</v>
+      </c>
+      <c r="C74">
+        <v>30</v>
+      </c>
+      <c r="D74" t="s">
+        <v>267</v>
+      </c>
+      <c r="E74">
+        <v>1998</v>
+      </c>
+      <c r="F74" t="s">
+        <v>268</v>
+      </c>
+      <c r="G74" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>46</v>
+      </c>
+      <c r="B75" t="s">
+        <v>267</v>
+      </c>
+      <c r="C75">
+        <v>42</v>
+      </c>
+      <c r="D75" t="s">
+        <v>267</v>
+      </c>
+      <c r="E75">
+        <v>2007</v>
+      </c>
+      <c r="F75" t="s">
+        <v>268</v>
+      </c>
+      <c r="G75" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
+        <v>45</v>
+      </c>
+      <c r="B76" t="s">
+        <v>267</v>
+      </c>
+      <c r="C76">
+        <v>36</v>
+      </c>
+      <c r="D76" t="s">
+        <v>267</v>
+      </c>
+      <c r="E76">
+        <v>2005</v>
+      </c>
+      <c r="F76" t="s">
+        <v>268</v>
+      </c>
+      <c r="G76" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
+        <v>47</v>
+      </c>
+      <c r="B77" t="s">
+        <v>267</v>
+      </c>
+      <c r="C77">
+        <v>42</v>
+      </c>
+      <c r="D77" t="s">
+        <v>267</v>
+      </c>
+      <c r="E77">
+        <v>2009</v>
+      </c>
+      <c r="F77" t="s">
+        <v>268</v>
+      </c>
+      <c r="G77" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
+        <v>47</v>
+      </c>
+      <c r="B78" t="s">
+        <v>267</v>
+      </c>
+      <c r="C78">
+        <v>34</v>
+      </c>
+      <c r="D78" t="s">
+        <v>267</v>
+      </c>
+      <c r="E78">
+        <v>2010</v>
+      </c>
+      <c r="F78" t="s">
+        <v>268</v>
+      </c>
+      <c r="G78" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
+        <v>248</v>
+      </c>
+      <c r="B79" t="s">
+        <v>267</v>
+      </c>
+      <c r="C79">
+        <v>40</v>
+      </c>
+      <c r="D79" t="s">
+        <v>267</v>
+      </c>
+      <c r="E79">
+        <v>2008</v>
+      </c>
+      <c r="F79" t="s">
+        <v>268</v>
+      </c>
+      <c r="G79" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>249</v>
+      </c>
+      <c r="B80" t="s">
+        <v>267</v>
+      </c>
+      <c r="C80">
+        <v>38</v>
+      </c>
+      <c r="D80" t="s">
+        <v>267</v>
+      </c>
+      <c r="E80">
+        <v>2011</v>
+      </c>
+      <c r="F80" t="s">
+        <v>268</v>
+      </c>
+      <c r="G80" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" t="s">
+        <v>267</v>
+      </c>
+      <c r="C81">
+        <v>3</v>
+      </c>
+      <c r="D81" t="s">
+        <v>267</v>
+      </c>
+      <c r="E81">
+        <v>2006</v>
+      </c>
+      <c r="F81" t="s">
+        <v>268</v>
+      </c>
+      <c r="G81" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>175</v>
+      </c>
+      <c r="B82" t="s">
+        <v>267</v>
+      </c>
+      <c r="C82">
+        <v>24</v>
+      </c>
+      <c r="D82" t="s">
+        <v>267</v>
+      </c>
+      <c r="E82">
+        <v>1992</v>
+      </c>
+      <c r="F82" t="s">
+        <v>268</v>
+      </c>
+      <c r="G82" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>253</v>
+      </c>
+      <c r="B83" t="s">
+        <v>267</v>
+      </c>
+      <c r="C83">
+        <v>6</v>
+      </c>
+      <c r="D83" t="s">
+        <v>267</v>
+      </c>
+      <c r="E83">
+        <v>1979</v>
+      </c>
+      <c r="F83" t="s">
+        <v>268</v>
+      </c>
+      <c r="G83" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>9</v>
+      </c>
+      <c r="B84" t="s">
+        <v>267</v>
+      </c>
+      <c r="C84">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s">
+        <v>267</v>
+      </c>
+      <c r="E84">
+        <v>2007</v>
+      </c>
+      <c r="F84" t="s">
+        <v>268</v>
+      </c>
+      <c r="G84" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>53</v>
+      </c>
+      <c r="B85" t="s">
+        <v>267</v>
+      </c>
+      <c r="C85">
+        <v>20</v>
+      </c>
+      <c r="D85" t="s">
+        <v>267</v>
+      </c>
+      <c r="E85">
+        <v>2007</v>
+      </c>
+      <c r="F85" t="s">
+        <v>268</v>
+      </c>
+      <c r="G85" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>171</v>
+      </c>
+      <c r="B86" t="s">
+        <v>267</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86" t="s">
+        <v>267</v>
+      </c>
+      <c r="E86">
+        <v>1991</v>
+      </c>
+      <c r="F86" t="s">
+        <v>268</v>
+      </c>
+      <c r="G86" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>243</v>
+      </c>
+      <c r="B87" t="s">
+        <v>267</v>
+      </c>
+      <c r="C87">
+        <v>12</v>
+      </c>
+      <c r="D87" t="s">
+        <v>267</v>
+      </c>
+      <c r="E87">
+        <v>2001</v>
+      </c>
+      <c r="F87" t="s">
+        <v>268</v>
+      </c>
+      <c r="G87" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>244</v>
+      </c>
+      <c r="B88" t="s">
+        <v>267</v>
+      </c>
+      <c r="C88">
+        <v>21</v>
+      </c>
+      <c r="D88" t="s">
+        <v>267</v>
+      </c>
+      <c r="E88">
+        <v>2002</v>
+      </c>
+      <c r="F88" t="s">
+        <v>268</v>
+      </c>
+      <c r="G88" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89" t="s">
+        <v>267</v>
+      </c>
+      <c r="C89">
+        <v>17</v>
+      </c>
+      <c r="D89" t="s">
+        <v>267</v>
+      </c>
+      <c r="E89">
+        <v>2004</v>
+      </c>
+      <c r="F89" t="s">
+        <v>268</v>
+      </c>
+      <c r="G89" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>245</v>
+      </c>
+      <c r="B90" t="s">
+        <v>267</v>
+      </c>
+      <c r="C90">
+        <v>41</v>
+      </c>
+      <c r="D90" t="s">
+        <v>267</v>
+      </c>
+      <c r="E90">
+        <v>2004</v>
+      </c>
+      <c r="F90" t="s">
+        <v>268</v>
+      </c>
+      <c r="G90" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" t="s">
+        <v>246</v>
+      </c>
+      <c r="B91" t="s">
+        <v>267</v>
+      </c>
+      <c r="C91">
+        <v>41</v>
+      </c>
+      <c r="D91" t="s">
+        <v>267</v>
+      </c>
+      <c r="E91">
+        <v>2005</v>
+      </c>
+      <c r="F91" t="s">
+        <v>268</v>
+      </c>
+      <c r="G91" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>167</v>
+      </c>
+      <c r="B92" t="s">
+        <v>267</v>
+      </c>
+      <c r="C92">
+        <v>15</v>
+      </c>
+      <c r="D92" t="s">
+        <v>267</v>
+      </c>
+      <c r="E92">
+        <v>1998</v>
+      </c>
+      <c r="F92" t="s">
+        <v>268</v>
+      </c>
+      <c r="G92" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>54</v>
+      </c>
+      <c r="B93" t="s">
+        <v>267</v>
+      </c>
+      <c r="C93">
+        <v>35</v>
+      </c>
+      <c r="D93" t="s">
+        <v>267</v>
+      </c>
+      <c r="E93">
+        <v>2009</v>
+      </c>
+      <c r="F93" t="s">
+        <v>268</v>
+      </c>
+      <c r="G93" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
+        <v>56</v>
+      </c>
+      <c r="B94" t="s">
+        <v>267</v>
+      </c>
+      <c r="C94">
+        <v>3</v>
+      </c>
+      <c r="D94" t="s">
+        <v>267</v>
+      </c>
+      <c r="E94">
+        <v>2005</v>
+      </c>
+      <c r="F94" t="s">
+        <v>268</v>
+      </c>
+      <c r="G94" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>250</v>
+      </c>
+      <c r="B95" t="s">
+        <v>267</v>
+      </c>
+      <c r="C95">
+        <v>6</v>
+      </c>
+      <c r="D95" t="s">
+        <v>267</v>
+      </c>
+      <c r="E95">
+        <v>2012</v>
+      </c>
+      <c r="F95" t="s">
+        <v>268</v>
+      </c>
+      <c r="G95" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>251</v>
+      </c>
+      <c r="B96" t="s">
+        <v>267</v>
+      </c>
+      <c r="C96">
+        <v>6</v>
+      </c>
+      <c r="D96" t="s">
+        <v>267</v>
+      </c>
+      <c r="E96">
+        <v>2010</v>
+      </c>
+      <c r="F96" t="s">
+        <v>268</v>
+      </c>
+      <c r="G96" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>252</v>
+      </c>
+      <c r="B97" t="s">
+        <v>267</v>
+      </c>
+      <c r="C97">
+        <v>6</v>
+      </c>
+      <c r="D97" t="s">
+        <v>267</v>
+      </c>
+      <c r="E97">
+        <v>2007</v>
+      </c>
+      <c r="F97" t="s">
+        <v>268</v>
+      </c>
+      <c r="G97" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" t="s">
+        <v>177</v>
+      </c>
+      <c r="B98" t="s">
+        <v>267</v>
+      </c>
+      <c r="C98">
+        <v>25</v>
+      </c>
+      <c r="D98" t="s">
+        <v>267</v>
+      </c>
+      <c r="E98">
+        <v>1994</v>
+      </c>
+      <c r="F98" t="s">
+        <v>268</v>
+      </c>
+      <c r="G98" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>178</v>
+      </c>
+      <c r="B99" t="s">
+        <v>267</v>
+      </c>
+      <c r="C99">
+        <v>26</v>
+      </c>
+      <c r="D99" t="s">
+        <v>267</v>
+      </c>
+      <c r="E99">
+        <v>1995</v>
+      </c>
+      <c r="F99" t="s">
+        <v>268</v>
+      </c>
+      <c r="G99" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
+        <v>179</v>
+      </c>
+      <c r="B100" t="s">
+        <v>267</v>
+      </c>
+      <c r="C100">
+        <v>26</v>
+      </c>
+      <c r="D100" t="s">
+        <v>267</v>
+      </c>
+      <c r="E100">
+        <v>1999</v>
+      </c>
+      <c r="F100" t="s">
+        <v>268</v>
+      </c>
+      <c r="G100" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" t="s">
+        <v>180</v>
+      </c>
+      <c r="B101" t="s">
+        <v>267</v>
+      </c>
+      <c r="C101">
+        <v>27</v>
+      </c>
+      <c r="D101" t="s">
+        <v>267</v>
+      </c>
+      <c r="E101">
+        <v>2004</v>
+      </c>
+      <c r="F101" t="s">
+        <v>268</v>
+      </c>
+      <c r="G101" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" t="s">
+        <v>221</v>
+      </c>
+      <c r="B102" t="s">
+        <v>267</v>
+      </c>
+      <c r="C102">
+        <v>16</v>
+      </c>
+      <c r="D102" t="s">
+        <v>267</v>
+      </c>
+      <c r="E102">
+        <v>2009</v>
+      </c>
+      <c r="F102" t="s">
+        <v>268</v>
+      </c>
+      <c r="G102" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" t="s">
+        <v>58</v>
+      </c>
+      <c r="B103" t="s">
+        <v>267</v>
+      </c>
+      <c r="C103">
+        <v>5</v>
+      </c>
+      <c r="D103" t="s">
+        <v>267</v>
+      </c>
+      <c r="E103">
+        <v>2002</v>
+      </c>
+      <c r="F103" t="s">
+        <v>268</v>
+      </c>
+      <c r="G103" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" t="s">
+        <v>60</v>
+      </c>
+      <c r="B104" t="s">
+        <v>267</v>
+      </c>
+      <c r="C104">
+        <v>12</v>
+      </c>
+      <c r="D104" t="s">
+        <v>267</v>
+      </c>
+      <c r="E104">
+        <v>2005</v>
+      </c>
+      <c r="F104" t="s">
+        <v>268</v>
+      </c>
+      <c r="G104" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" t="s">
+        <v>64</v>
+      </c>
+      <c r="B105" t="s">
+        <v>267</v>
+      </c>
+      <c r="C105">
+        <v>3</v>
+      </c>
+      <c r="D105" t="s">
+        <v>267</v>
+      </c>
+      <c r="E105">
+        <v>2008</v>
+      </c>
+      <c r="F105" t="s">
+        <v>268</v>
+      </c>
+      <c r="G105" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" t="s">
+        <v>225</v>
+      </c>
+      <c r="B106" t="s">
+        <v>267</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106" t="s">
+        <v>267</v>
+      </c>
+      <c r="E106">
+        <v>1959</v>
+      </c>
+      <c r="F106" t="s">
+        <v>268</v>
+      </c>
+      <c r="G106" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" t="s">
+        <v>119</v>
+      </c>
+      <c r="B107" t="s">
+        <v>267</v>
+      </c>
+      <c r="C107">
+        <v>11</v>
+      </c>
+      <c r="D107" t="s">
+        <v>267</v>
+      </c>
+      <c r="E107">
+        <v>1970</v>
+      </c>
+      <c r="F107" t="s">
+        <v>268</v>
+      </c>
+      <c r="G107" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" t="s">
+        <v>123</v>
+      </c>
+      <c r="B108" t="s">
+        <v>267</v>
+      </c>
+      <c r="C108">
+        <v>11</v>
+      </c>
+      <c r="D108" t="s">
+        <v>267</v>
+      </c>
+      <c r="E108">
+        <v>1973</v>
+      </c>
+      <c r="F108" t="s">
+        <v>268</v>
+      </c>
+      <c r="G108" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" t="s">
+        <v>66</v>
+      </c>
+      <c r="B109" t="s">
+        <v>267</v>
+      </c>
+      <c r="C109">
+        <v>17</v>
+      </c>
+      <c r="D109" t="s">
+        <v>267</v>
+      </c>
+      <c r="E109">
+        <v>2007</v>
+      </c>
+      <c r="F109" t="s">
+        <v>268</v>
+      </c>
+      <c r="G109" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" t="s">
+        <v>115</v>
+      </c>
+      <c r="B110" t="s">
+        <v>267</v>
+      </c>
+      <c r="C110">
+        <v>2</v>
+      </c>
+      <c r="D110" t="s">
+        <v>267</v>
+      </c>
+      <c r="E110">
+        <v>1968</v>
+      </c>
+      <c r="F110" t="s">
+        <v>268</v>
+      </c>
+      <c r="G110" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
+        <v>26</v>
+      </c>
+      <c r="B111" t="s">
+        <v>267</v>
+      </c>
+      <c r="C111">
+        <v>22</v>
+      </c>
+      <c r="D111" t="s">
+        <v>267</v>
+      </c>
+      <c r="E111">
+        <v>2009</v>
+      </c>
+      <c r="F111" t="s">
+        <v>268</v>
+      </c>
+      <c r="G111" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" t="s">
+        <v>140</v>
+      </c>
+      <c r="B112" t="s">
+        <v>267</v>
+      </c>
+      <c r="C112">
+        <v>16</v>
+      </c>
+      <c r="D112" t="s">
+        <v>267</v>
+      </c>
+      <c r="E112">
+        <v>1984</v>
+      </c>
+      <c r="F112" t="s">
+        <v>268</v>
+      </c>
+      <c r="G112" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>18</v>
+      </c>
+      <c r="B113" t="s">
+        <v>267</v>
+      </c>
+      <c r="C113">
+        <v>25</v>
+      </c>
+      <c r="D113" t="s">
+        <v>267</v>
+      </c>
+      <c r="E113">
+        <v>2004</v>
+      </c>
+      <c r="F113" t="s">
+        <v>268</v>
+      </c>
+      <c r="G113" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" t="s">
+        <v>157</v>
+      </c>
+      <c r="B114" t="s">
+        <v>267</v>
+      </c>
+      <c r="C114">
+        <v>5</v>
+      </c>
+      <c r="D114" t="s">
+        <v>267</v>
+      </c>
+      <c r="E114">
+        <v>1986</v>
+      </c>
+      <c r="F114" t="s">
+        <v>268</v>
+      </c>
+      <c r="G114" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
+        <v>229</v>
+      </c>
+      <c r="B115" t="s">
+        <v>267</v>
+      </c>
+      <c r="C115">
+        <v>3</v>
+      </c>
+      <c r="D115" t="s">
+        <v>267</v>
+      </c>
+      <c r="E115">
+        <v>2010</v>
+      </c>
+      <c r="F115" t="s">
+        <v>268</v>
+      </c>
+      <c r="G115" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" t="s">
+        <v>185</v>
+      </c>
+      <c r="B116" t="s">
+        <v>267</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+      <c r="D116" t="s">
+        <v>267</v>
+      </c>
+      <c r="E116">
+        <v>1994</v>
+      </c>
+      <c r="F116" t="s">
+        <v>268</v>
+      </c>
+      <c r="G116" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" t="s">
+        <v>197</v>
+      </c>
+      <c r="B117" t="s">
+        <v>267</v>
+      </c>
+      <c r="C117">
+        <v>8</v>
+      </c>
+      <c r="D117" t="s">
+        <v>267</v>
+      </c>
+      <c r="E117">
+        <v>1997</v>
+      </c>
+      <c r="F117" t="s">
+        <v>268</v>
+      </c>
+      <c r="G117" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" t="s">
+        <v>131</v>
+      </c>
+      <c r="B118" t="s">
+        <v>267</v>
+      </c>
+      <c r="C118">
+        <v>6</v>
+      </c>
+      <c r="D118" t="s">
+        <v>267</v>
+      </c>
+      <c r="E118">
+        <v>1985</v>
+      </c>
+      <c r="F118" t="s">
+        <v>268</v>
+      </c>
+      <c r="G118" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" t="s">
+        <v>69</v>
+      </c>
+      <c r="B119" t="s">
+        <v>267</v>
+      </c>
+      <c r="C119">
+        <v>28</v>
+      </c>
+      <c r="D119" t="s">
+        <v>267</v>
+      </c>
+      <c r="E119">
+        <v>2006</v>
+      </c>
+      <c r="F119" t="s">
+        <v>268</v>
+      </c>
+      <c r="G119" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" t="s">
+        <v>67</v>
+      </c>
+      <c r="B120" t="s">
+        <v>267</v>
+      </c>
+      <c r="C120">
+        <v>3</v>
+      </c>
+      <c r="D120" t="s">
+        <v>267</v>
+      </c>
+      <c r="E120">
+        <v>2004</v>
+      </c>
+      <c r="F120" t="s">
+        <v>268</v>
+      </c>
+      <c r="G120" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" t="s">
+        <v>152</v>
+      </c>
+      <c r="B121" t="s">
+        <v>267</v>
+      </c>
+      <c r="C121">
+        <v>30</v>
+      </c>
+      <c r="D121" t="s">
+        <v>267</v>
+      </c>
+      <c r="E121">
+        <v>1993</v>
+      </c>
+      <c r="F121" t="s">
+        <v>268</v>
+      </c>
+      <c r="G121" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" t="s">
+        <v>153</v>
+      </c>
+      <c r="B122" t="s">
+        <v>267</v>
+      </c>
+      <c r="C122">
+        <v>30</v>
+      </c>
+      <c r="D122" t="s">
+        <v>267</v>
+      </c>
+      <c r="E122">
+        <v>1996</v>
+      </c>
+      <c r="F122" t="s">
+        <v>268</v>
+      </c>
+      <c r="G122" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" t="s">
+        <v>41</v>
+      </c>
+      <c r="B123" t="s">
+        <v>267</v>
+      </c>
+      <c r="C123">
+        <v>28</v>
+      </c>
+      <c r="D123" t="s">
+        <v>267</v>
+      </c>
+      <c r="E123">
+        <v>1997</v>
+      </c>
+      <c r="F123" t="s">
+        <v>268</v>
+      </c>
+      <c r="G123" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" t="s">
+        <v>154</v>
+      </c>
+      <c r="B124" t="s">
+        <v>267</v>
+      </c>
+      <c r="C124">
+        <v>34</v>
+      </c>
+      <c r="D124" t="s">
+        <v>267</v>
+      </c>
+      <c r="E124">
+        <v>2000</v>
+      </c>
+      <c r="F124" t="s">
+        <v>268</v>
+      </c>
+      <c r="G124" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" t="s">
+        <v>17</v>
+      </c>
+      <c r="B125" t="s">
+        <v>267</v>
+      </c>
+      <c r="C125">
+        <v>11</v>
+      </c>
+      <c r="D125" t="s">
+        <v>267</v>
+      </c>
+      <c r="E125">
+        <v>1998</v>
+      </c>
+      <c r="F125" t="s">
+        <v>268</v>
+      </c>
+      <c r="G125" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" t="s">
+        <v>168</v>
+      </c>
+      <c r="B126" t="s">
+        <v>267</v>
+      </c>
+      <c r="C126">
+        <v>3</v>
+      </c>
+      <c r="D126" t="s">
+        <v>267</v>
+      </c>
+      <c r="E126">
+        <v>2003</v>
+      </c>
+      <c r="F126" t="s">
+        <v>268</v>
+      </c>
+      <c r="G126" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="A127" t="s">
+        <v>62</v>
+      </c>
+      <c r="B127" t="s">
+        <v>267</v>
+      </c>
+      <c r="C127">
+        <v>30</v>
+      </c>
+      <c r="D127" t="s">
+        <v>267</v>
+      </c>
+      <c r="E127">
+        <v>2010</v>
+      </c>
+      <c r="F127" t="s">
+        <v>268</v>
+      </c>
+      <c r="G127" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" t="s">
+        <v>71</v>
+      </c>
+      <c r="B128" t="s">
+        <v>267</v>
+      </c>
+      <c r="C128">
+        <v>18</v>
+      </c>
+      <c r="D128" t="s">
+        <v>267</v>
+      </c>
+      <c r="E128">
+        <v>2007</v>
+      </c>
+      <c r="F128" t="s">
+        <v>268</v>
+      </c>
+      <c r="G128" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" t="s">
+        <v>183</v>
+      </c>
+      <c r="B129" t="s">
+        <v>267</v>
+      </c>
+      <c r="C129">
+        <v>5</v>
+      </c>
+      <c r="D129" t="s">
+        <v>267</v>
+      </c>
+      <c r="E129">
+        <v>1993</v>
+      </c>
+      <c r="F129" t="s">
+        <v>268</v>
+      </c>
+      <c r="G129" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" t="s">
+        <v>232</v>
+      </c>
+      <c r="B130" t="s">
+        <v>267</v>
+      </c>
+      <c r="C130">
+        <v>18</v>
+      </c>
+      <c r="D130" t="s">
+        <v>267</v>
+      </c>
+      <c r="E130">
+        <v>2010</v>
+      </c>
+      <c r="F130" t="s">
+        <v>268</v>
+      </c>
+      <c r="G130" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" t="s">
+        <v>11</v>
+      </c>
+      <c r="B131" t="s">
+        <v>267</v>
+      </c>
+      <c r="C131">
+        <v>6</v>
+      </c>
+      <c r="D131" t="s">
+        <v>267</v>
+      </c>
+      <c r="E131">
+        <v>1975</v>
+      </c>
+      <c r="F131" t="s">
+        <v>268</v>
+      </c>
+      <c r="G131" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" t="s">
+        <v>190</v>
+      </c>
+      <c r="B132" t="s">
+        <v>267</v>
+      </c>
+      <c r="C132">
+        <v>2</v>
+      </c>
+      <c r="D132" t="s">
+        <v>267</v>
+      </c>
+      <c r="E132">
+        <v>1995</v>
+      </c>
+      <c r="F132" t="s">
+        <v>268</v>
+      </c>
+      <c r="G132" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" t="s">
+        <v>144</v>
+      </c>
+      <c r="B133" t="s">
+        <v>267</v>
+      </c>
+      <c r="C133">
+        <v>4</v>
+      </c>
+      <c r="D133" t="s">
+        <v>267</v>
+      </c>
+      <c r="E133">
+        <v>1985</v>
+      </c>
+      <c r="F133" t="s">
+        <v>268</v>
+      </c>
+      <c r="G133" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" t="s">
+        <v>49</v>
+      </c>
+      <c r="B134" t="s">
+        <v>267</v>
+      </c>
+      <c r="C134">
+        <v>3</v>
+      </c>
+      <c r="D134" t="s">
+        <v>267</v>
+      </c>
+      <c r="E134">
+        <v>2009</v>
+      </c>
+      <c r="F134" t="s">
+        <v>268</v>
+      </c>
+      <c r="G134" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
+      <c r="A135" t="s">
+        <v>201</v>
+      </c>
+      <c r="B135" t="s">
+        <v>267</v>
+      </c>
+      <c r="C135">
+        <v>3</v>
+      </c>
+      <c r="D135" t="s">
+        <v>267</v>
+      </c>
+      <c r="E135">
+        <v>1998</v>
+      </c>
+      <c r="F135" t="s">
+        <v>268</v>
+      </c>
+      <c r="G135" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" t="s">
+        <v>136</v>
+      </c>
+      <c r="B136" t="s">
+        <v>267</v>
+      </c>
+      <c r="C136">
+        <v>5</v>
+      </c>
+      <c r="D136" t="s">
+        <v>267</v>
+      </c>
+      <c r="E136">
+        <v>1983</v>
+      </c>
+      <c r="F136" t="s">
+        <v>268</v>
+      </c>
+      <c r="G136" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
+      <c r="A137" t="s">
+        <v>63</v>
+      </c>
+      <c r="B137" t="s">
+        <v>267</v>
+      </c>
+      <c r="C137">
+        <v>35</v>
+      </c>
+      <c r="D137" t="s">
+        <v>267</v>
+      </c>
+      <c r="E137">
+        <v>2006</v>
+      </c>
+      <c r="F137" t="s">
+        <v>268</v>
+      </c>
+      <c r="G137" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" t="s">
+        <v>198</v>
+      </c>
+      <c r="B138" t="s">
+        <v>267</v>
+      </c>
+      <c r="C138">
+        <v>3</v>
+      </c>
+      <c r="D138" t="s">
+        <v>267</v>
+      </c>
+      <c r="E138">
+        <v>1997</v>
+      </c>
+      <c r="F138" t="s">
+        <v>268</v>
+      </c>
+      <c r="G138" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="A139" t="s">
+        <v>242</v>
+      </c>
+      <c r="B139" t="s">
+        <v>267</v>
+      </c>
+      <c r="C139">
+        <v>2</v>
+      </c>
+      <c r="D139" t="s">
+        <v>267</v>
+      </c>
+      <c r="E139">
+        <v>2013</v>
+      </c>
+      <c r="F139" t="s">
+        <v>268</v>
+      </c>
+      <c r="G139" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" t="s">
+        <v>72</v>
+      </c>
+      <c r="B140" t="s">
+        <v>267</v>
+      </c>
+      <c r="C140">
+        <v>2</v>
+      </c>
+      <c r="D140" t="s">
+        <v>267</v>
+      </c>
+      <c r="E140">
+        <v>2011</v>
+      </c>
+      <c r="F140" t="s">
+        <v>268</v>
+      </c>
+      <c r="G140" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" t="s">
+        <v>235</v>
+      </c>
+      <c r="B141" t="s">
+        <v>267</v>
+      </c>
+      <c r="C141">
+        <v>40</v>
+      </c>
+      <c r="D141" t="s">
+        <v>267</v>
+      </c>
+      <c r="E141">
+        <v>2009</v>
+      </c>
+      <c r="F141" t="s">
+        <v>268</v>
+      </c>
+      <c r="G141" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c r="A142" t="s">
+        <v>237</v>
+      </c>
+      <c r="B142" t="s">
+        <v>267</v>
+      </c>
+      <c r="C142">
+        <v>40</v>
+      </c>
+      <c r="D142" t="s">
+        <v>267</v>
+      </c>
+      <c r="E142">
+        <v>2010</v>
+      </c>
+      <c r="F142" t="s">
+        <v>268</v>
+      </c>
+      <c r="G142" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
+      <c r="A143" t="s">
+        <v>6</v>
+      </c>
+      <c r="B143" t="s">
+        <v>267</v>
+      </c>
+      <c r="C143">
+        <v>16</v>
+      </c>
+      <c r="D143" t="s">
+        <v>267</v>
+      </c>
+      <c r="E143">
+        <v>2007</v>
+      </c>
+      <c r="F143" t="s">
+        <v>268</v>
+      </c>
+      <c r="G143" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" t="s">
+        <v>76</v>
+      </c>
+      <c r="B144" t="s">
+        <v>267</v>
+      </c>
+      <c r="C144">
+        <v>11</v>
+      </c>
+      <c r="D144" t="s">
+        <v>267</v>
+      </c>
+      <c r="E144">
+        <v>2006</v>
+      </c>
+      <c r="F144" t="s">
+        <v>268</v>
+      </c>
+      <c r="G144" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" t="s">
+        <v>73</v>
+      </c>
+      <c r="B145" t="s">
+        <v>267</v>
+      </c>
+      <c r="C145">
+        <v>11</v>
+      </c>
+      <c r="D145" t="s">
+        <v>267</v>
+      </c>
+      <c r="E145">
+        <v>2005</v>
+      </c>
+      <c r="F145" t="s">
+        <v>268</v>
+      </c>
+      <c r="G145" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" t="s">
+        <v>161</v>
+      </c>
+      <c r="B146" t="s">
+        <v>267</v>
+      </c>
+      <c r="C146">
+        <v>13</v>
+      </c>
+      <c r="D146" t="s">
+        <v>267</v>
+      </c>
+      <c r="E146">
+        <v>1989</v>
+      </c>
+      <c r="F146" t="s">
+        <v>268</v>
+      </c>
+      <c r="G146" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" t="s">
+        <v>191</v>
+      </c>
+      <c r="B147" t="s">
+        <v>267</v>
+      </c>
+      <c r="C147">
+        <v>6</v>
+      </c>
+      <c r="D147" t="s">
+        <v>267</v>
+      </c>
+      <c r="E147">
+        <v>1993</v>
+      </c>
+      <c r="F147" t="s">
+        <v>268</v>
+      </c>
+      <c r="G147" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" t="s">
+        <v>159</v>
+      </c>
+      <c r="B148" t="s">
+        <v>267</v>
+      </c>
+      <c r="C148">
+        <v>5</v>
+      </c>
+      <c r="D148" t="s">
+        <v>267</v>
+      </c>
+      <c r="E148">
+        <v>1988</v>
+      </c>
+      <c r="F148" t="s">
+        <v>268</v>
+      </c>
+      <c r="G148" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149" t="s">
+        <v>57</v>
+      </c>
+      <c r="B149" t="s">
+        <v>267</v>
+      </c>
+      <c r="C149">
+        <v>3</v>
+      </c>
+      <c r="D149" t="s">
+        <v>267</v>
+      </c>
+      <c r="E149">
+        <v>2002</v>
+      </c>
+      <c r="F149" t="s">
+        <v>268</v>
+      </c>
+      <c r="G149" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" t="s">
+        <v>77</v>
+      </c>
+      <c r="B150" t="s">
+        <v>267</v>
+      </c>
+      <c r="C150">
+        <v>30</v>
+      </c>
+      <c r="D150" t="s">
+        <v>267</v>
+      </c>
+      <c r="E150">
+        <v>2012</v>
+      </c>
+      <c r="F150" t="s">
+        <v>268</v>
+      </c>
+      <c r="G150" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" t="s">
+        <v>78</v>
+      </c>
+      <c r="B151" t="s">
+        <v>267</v>
+      </c>
+      <c r="C151">
+        <v>24</v>
+      </c>
+      <c r="D151" t="s">
+        <v>267</v>
+      </c>
+      <c r="E151">
+        <v>2011</v>
+      </c>
+      <c r="F151" t="s">
+        <v>268</v>
+      </c>
+      <c r="G151" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" t="s">
+        <v>193</v>
+      </c>
+      <c r="B152" t="s">
+        <v>267</v>
+      </c>
+      <c r="C152">
+        <v>41</v>
+      </c>
+      <c r="D152" t="s">
+        <v>267</v>
+      </c>
+      <c r="E152">
+        <v>1995</v>
+      </c>
+      <c r="F152" t="s">
+        <v>268</v>
+      </c>
+      <c r="G152" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" t="s">
+        <v>223</v>
+      </c>
+      <c r="B153" t="s">
+        <v>267</v>
+      </c>
+      <c r="C153">
+        <v>11</v>
+      </c>
+      <c r="D153" t="s">
+        <v>267</v>
+      </c>
+      <c r="E153">
+        <v>2008</v>
+      </c>
+      <c r="F153" t="s">
+        <v>268</v>
+      </c>
+      <c r="G153" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
+      <c r="A154" t="s">
+        <v>51</v>
+      </c>
+      <c r="B154" t="s">
+        <v>267</v>
+      </c>
+      <c r="C154">
+        <v>4</v>
+      </c>
+      <c r="D154" t="s">
+        <v>267</v>
+      </c>
+      <c r="E154">
+        <v>2008</v>
+      </c>
+      <c r="F154" t="s">
+        <v>268</v>
+      </c>
+      <c r="G154" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" t="s">
+        <v>117</v>
+      </c>
+      <c r="B155" t="s">
+        <v>267</v>
+      </c>
+      <c r="C155">
+        <v>5</v>
+      </c>
+      <c r="D155" t="s">
+        <v>267</v>
+      </c>
+      <c r="E155">
+        <v>1970</v>
+      </c>
+      <c r="F155" t="s">
+        <v>268</v>
+      </c>
+      <c r="G155" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7">
+      <c r="A156" t="s">
+        <v>80</v>
+      </c>
+      <c r="B156" t="s">
+        <v>267</v>
+      </c>
+      <c r="C156">
+        <v>21</v>
+      </c>
+      <c r="D156" t="s">
+        <v>267</v>
+      </c>
+      <c r="E156">
+        <v>2010</v>
+      </c>
+      <c r="F156" t="s">
+        <v>268</v>
+      </c>
+      <c r="G156" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
+      <c r="A157" t="s">
+        <v>81</v>
+      </c>
+      <c r="B157" t="s">
+        <v>267</v>
+      </c>
+      <c r="C157">
+        <v>20</v>
+      </c>
+      <c r="D157" t="s">
+        <v>267</v>
+      </c>
+      <c r="E157">
+        <v>2004</v>
+      </c>
+      <c r="F157" t="s">
+        <v>268</v>
+      </c>
+      <c r="G157" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7">
+      <c r="A158" t="s">
+        <v>21</v>
+      </c>
+      <c r="B158" t="s">
+        <v>267</v>
+      </c>
+      <c r="C158">
+        <v>2</v>
+      </c>
+      <c r="D158" t="s">
+        <v>267</v>
+      </c>
+      <c r="E158">
+        <v>1966</v>
+      </c>
+      <c r="F158" t="s">
+        <v>268</v>
+      </c>
+      <c r="G158" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" t="s">
+        <v>23</v>
+      </c>
+      <c r="B159" t="s">
+        <v>267</v>
+      </c>
+      <c r="C159">
+        <v>15</v>
+      </c>
+      <c r="D159" t="s">
+        <v>267</v>
+      </c>
+      <c r="E159">
+        <v>1997</v>
+      </c>
+      <c r="F159" t="s">
+        <v>268</v>
+      </c>
+      <c r="G159" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" t="s">
+        <v>19</v>
+      </c>
+      <c r="B160" t="s">
+        <v>267</v>
+      </c>
+      <c r="C160">
+        <v>30</v>
+      </c>
+      <c r="D160" t="s">
+        <v>267</v>
+      </c>
+      <c r="E160">
+        <v>2004</v>
+      </c>
+      <c r="F160" t="s">
+        <v>268</v>
+      </c>
+      <c r="G160" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
+      <c r="A161" t="s">
+        <v>202</v>
+      </c>
+      <c r="B161" t="s">
+        <v>267</v>
+      </c>
+      <c r="C161">
+        <v>2</v>
+      </c>
+      <c r="D161" t="s">
+        <v>267</v>
+      </c>
+      <c r="E161">
+        <v>1998</v>
+      </c>
+      <c r="F161" t="s">
+        <v>268</v>
+      </c>
+      <c r="G161" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
+      <c r="A162" t="s">
+        <v>37</v>
+      </c>
+      <c r="B162" t="s">
+        <v>267</v>
+      </c>
+      <c r="C162">
+        <v>7</v>
+      </c>
+      <c r="D162" t="s">
+        <v>267</v>
+      </c>
+      <c r="E162">
+        <v>2003</v>
+      </c>
+      <c r="F162" t="s">
+        <v>268</v>
+      </c>
+      <c r="G162" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7">
+      <c r="A163" t="s">
+        <v>90</v>
+      </c>
+      <c r="B163" t="s">
+        <v>267</v>
+      </c>
+      <c r="C163">
+        <v>2</v>
+      </c>
+      <c r="D163" t="s">
+        <v>267</v>
+      </c>
+      <c r="E163">
+        <v>1930</v>
+      </c>
+      <c r="F163" t="s">
+        <v>268</v>
+      </c>
+      <c r="G163" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7">
+      <c r="A164" t="s">
+        <v>108</v>
+      </c>
+      <c r="B164" t="s">
+        <v>267</v>
+      </c>
+      <c r="C164">
+        <v>6</v>
+      </c>
+      <c r="D164" t="s">
+        <v>267</v>
+      </c>
+      <c r="E164">
+        <v>1962</v>
+      </c>
+      <c r="F164" t="s">
+        <v>268</v>
+      </c>
+      <c r="G164" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7">
+      <c r="A165" t="s">
+        <v>238</v>
+      </c>
+      <c r="B165" t="s">
+        <v>267</v>
+      </c>
+      <c r="C165">
+        <v>28</v>
+      </c>
+      <c r="D165" t="s">
+        <v>267</v>
+      </c>
+      <c r="E165">
+        <v>2010</v>
+      </c>
+      <c r="F165" t="s">
+        <v>268</v>
+      </c>
+      <c r="G165" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7">
+      <c r="A166" t="s">
+        <v>138</v>
+      </c>
+      <c r="B166" t="s">
+        <v>267</v>
+      </c>
+      <c r="C166">
+        <v>5</v>
+      </c>
+      <c r="D166" t="s">
+        <v>267</v>
+      </c>
+      <c r="E166">
+        <v>1983</v>
+      </c>
+      <c r="F166" t="s">
+        <v>268</v>
+      </c>
+      <c r="G166" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7">
+      <c r="A167" t="s">
+        <v>218</v>
+      </c>
+      <c r="B167" t="s">
+        <v>267</v>
+      </c>
+      <c r="C167">
+        <v>3</v>
+      </c>
+      <c r="D167" t="s">
+        <v>267</v>
+      </c>
+      <c r="E167">
+        <v>1999</v>
+      </c>
+      <c r="F167" t="s">
+        <v>268</v>
+      </c>
+      <c r="G167" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7">
+      <c r="A168" t="s">
+        <v>257</v>
+      </c>
+      <c r="B168" t="s">
+        <v>267</v>
+      </c>
+      <c r="C168">
+        <v>2</v>
+      </c>
+      <c r="D168" t="s">
+        <v>267</v>
+      </c>
+      <c r="E168">
+        <v>1949</v>
+      </c>
+      <c r="F168" t="s">
+        <v>268</v>
+      </c>
+      <c r="G168" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7">
+      <c r="A169" t="s">
+        <v>15</v>
+      </c>
+      <c r="B169" t="s">
+        <v>267</v>
+      </c>
+      <c r="C169">
+        <v>6</v>
+      </c>
+      <c r="D169" t="s">
+        <v>267</v>
+      </c>
+      <c r="E169">
+        <v>1954</v>
+      </c>
+      <c r="F169" t="s">
+        <v>268</v>
+      </c>
+      <c r="G169" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7">
+      <c r="A170" t="s">
+        <v>181</v>
+      </c>
+      <c r="B170" t="s">
+        <v>267</v>
+      </c>
+      <c r="C170">
+        <v>4</v>
+      </c>
+      <c r="D170" t="s">
+        <v>267</v>
+      </c>
+      <c r="E170">
+        <v>1992</v>
+      </c>
+      <c r="F170" t="s">
+        <v>268</v>
+      </c>
+      <c r="G170" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7">
+      <c r="A171" t="s">
+        <v>186</v>
+      </c>
+      <c r="B171" t="s">
+        <v>267</v>
+      </c>
+      <c r="C171">
+        <v>2</v>
+      </c>
+      <c r="D171" t="s">
+        <v>267</v>
+      </c>
+      <c r="E171">
+        <v>1994</v>
+      </c>
+      <c r="F171" t="s">
+        <v>268</v>
+      </c>
+      <c r="G171" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7">
+      <c r="A172" t="s">
+        <v>125</v>
+      </c>
+      <c r="B172" t="s">
+        <v>267</v>
+      </c>
+      <c r="C172">
+        <v>5</v>
+      </c>
+      <c r="D172" t="s">
+        <v>267</v>
+      </c>
+      <c r="E172">
+        <v>1977</v>
+      </c>
+      <c r="F172" t="s">
+        <v>268</v>
+      </c>
+      <c r="G172" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7">
+      <c r="A173" t="s">
+        <v>239</v>
+      </c>
+      <c r="B173" t="s">
+        <v>267</v>
+      </c>
+      <c r="C173">
+        <v>26</v>
+      </c>
+      <c r="D173" t="s">
+        <v>267</v>
+      </c>
+      <c r="E173">
+        <v>2010</v>
+      </c>
+      <c r="F173" t="s">
+        <v>268</v>
+      </c>
+      <c r="G173" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7">
+      <c r="A174" t="s">
+        <v>109</v>
+      </c>
+      <c r="B174" t="s">
+        <v>267</v>
+      </c>
+      <c r="C174">
+        <v>16</v>
+      </c>
+      <c r="D174" t="s">
+        <v>267</v>
+      </c>
+      <c r="E174">
+        <v>1968</v>
+      </c>
+      <c r="F174" t="s">
+        <v>268</v>
+      </c>
+      <c r="G174" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7">
+      <c r="A175" t="s">
+        <v>52</v>
+      </c>
+      <c r="B175" t="s">
+        <v>267</v>
+      </c>
+      <c r="C175">
+        <v>13</v>
+      </c>
+      <c r="D175" t="s">
+        <v>267</v>
+      </c>
+      <c r="E175">
+        <v>2008</v>
+      </c>
+      <c r="F175" t="s">
+        <v>268</v>
+      </c>
+      <c r="G175" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7">
+      <c r="A176" t="s">
+        <v>121</v>
+      </c>
+      <c r="B176" t="s">
+        <v>267</v>
+      </c>
+      <c r="C176">
+        <v>5</v>
+      </c>
+      <c r="D176" t="s">
+        <v>267</v>
+      </c>
+      <c r="E176">
+        <v>1972</v>
+      </c>
+      <c r="F176" t="s">
+        <v>268</v>
+      </c>
+      <c r="G176" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7">
+      <c r="A177" t="s">
+        <v>82</v>
+      </c>
+      <c r="B177" t="s">
+        <v>267</v>
+      </c>
+      <c r="C177">
+        <v>10</v>
+      </c>
+      <c r="D177" t="s">
+        <v>267</v>
+      </c>
+      <c r="E177">
+        <v>2006</v>
+      </c>
+      <c r="F177" t="s">
+        <v>268</v>
+      </c>
+      <c r="G177" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7">
+      <c r="A178" t="s">
+        <v>83</v>
+      </c>
+      <c r="B178" t="s">
+        <v>267</v>
+      </c>
+      <c r="C178">
+        <v>2</v>
+      </c>
+      <c r="D178" t="s">
+        <v>267</v>
+      </c>
+      <c r="E178">
+        <v>2000</v>
+      </c>
+      <c r="F178" t="s">
+        <v>268</v>
+      </c>
+      <c r="G178" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7">
+      <c r="A179" t="s">
+        <v>84</v>
+      </c>
+      <c r="B179" t="s">
+        <v>267</v>
+      </c>
+      <c r="C179">
+        <v>3</v>
+      </c>
+      <c r="D179" t="s">
+        <v>267</v>
+      </c>
+      <c r="E179">
+        <v>2005</v>
+      </c>
+      <c r="F179" t="s">
+        <v>268</v>
+      </c>
+      <c r="G179" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7">
+      <c r="A180" t="s">
+        <v>86</v>
+      </c>
+      <c r="B180" t="s">
+        <v>267</v>
+      </c>
+      <c r="C180">
+        <v>10</v>
+      </c>
+      <c r="D180" t="s">
+        <v>267</v>
+      </c>
+      <c r="E180">
+        <v>2009</v>
+      </c>
+      <c r="F180" t="s">
+        <v>268</v>
+      </c>
+      <c r="G180" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7">
+      <c r="A181" t="s">
+        <v>255</v>
+      </c>
+      <c r="B181" t="s">
+        <v>267</v>
+      </c>
+      <c r="C181">
+        <v>10</v>
+      </c>
+      <c r="D181" t="s">
+        <v>267</v>
+      </c>
+      <c r="E181">
+        <v>2010</v>
+      </c>
+      <c r="F181" t="s">
+        <v>268</v>
+      </c>
+      <c r="G181" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:C181">
+    <sortCondition ref="A2:A181"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added most of the programming stuff
</commit_message>
<xml_diff>
--- a/latex/robotsDOF.xlsx
+++ b/latex/robotsDOF.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14040" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="13980" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -5712,7 +5712,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>